<commit_message>
Add content to data table
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CongratulationsGenerator\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4864B27-1EFF-488A-A09C-673504D863DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Recipients" sheetId="1" r:id="rId1"/>
+    <sheet name="Wishes" sheetId="2" r:id="rId2"/>
+    <sheet name="Preferences" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,14 +26,133 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+  <si>
+    <t>Коротков Иван</t>
+  </si>
+  <si>
+    <t>м</t>
+  </si>
+  <si>
+    <t>Зуев Олег</t>
+  </si>
+  <si>
+    <t>Калинин Владимир</t>
+  </si>
+  <si>
+    <t>Филатова Полина</t>
+  </si>
+  <si>
+    <t>Вотинова Елизавета</t>
+  </si>
+  <si>
+    <t>ж</t>
+  </si>
+  <si>
+    <t>Здоровье</t>
+  </si>
+  <si>
+    <t>Учеба</t>
+  </si>
+  <si>
+    <t>Отношения</t>
+  </si>
+  <si>
+    <t>Карьера</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Пол</t>
+  </si>
+  <si>
+    <t>долгих лет жизни</t>
+  </si>
+  <si>
+    <t>отменного здоровья</t>
+  </si>
+  <si>
+    <t>отличной учебы</t>
+  </si>
+  <si>
+    <t>отличных оценок</t>
+  </si>
+  <si>
+    <t>успехов в учебе</t>
+  </si>
+  <si>
+    <t>счастья в любви</t>
+  </si>
+  <si>
+    <t>счастья в отношениях</t>
+  </si>
+  <si>
+    <t>счастливой семейной жизни</t>
+  </si>
+  <si>
+    <t>недюжиной силы</t>
+  </si>
+  <si>
+    <t>успехов в спорте</t>
+  </si>
+  <si>
+    <t>успехов во всех начинаниях</t>
+  </si>
+  <si>
+    <t>удачи</t>
+  </si>
+  <si>
+    <t>, чтобы все удавалось с первого раза</t>
+  </si>
+  <si>
+    <t>успехов</t>
+  </si>
+  <si>
+    <t>побед во всех начинаниях</t>
+  </si>
+  <si>
+    <t>Счастье и успех</t>
+  </si>
+  <si>
+    <t>счастья</t>
+  </si>
+  <si>
+    <t>продвижения по карьерной лестнице</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>Consolas</t>
+  </si>
+  <si>
+    <t>Congratulations letter template.dotx</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +458,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E8FAB2-6777-4297-A3DB-429CB167C58E}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBA24F2-5634-40F0-B3CB-5E5C0BF1A3A9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more recipients to data table
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CongratulationsGenerator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4864B27-1EFF-488A-A09C-673504D863DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7033F89-5222-4E2C-AC00-493AB12317B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipients" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Коротков Иван</t>
   </si>
@@ -104,9 +104,6 @@
     <t>удачи</t>
   </si>
   <si>
-    <t>, чтобы все удавалось с первого раза</t>
-  </si>
-  <si>
     <t>успехов</t>
   </si>
   <si>
@@ -132,6 +129,33 @@
   </si>
   <si>
     <t>Congratulations letter template.dotx</t>
+  </si>
+  <si>
+    <t>Оптимус Прайм</t>
+  </si>
+  <si>
+    <t>трансформер</t>
+  </si>
+  <si>
+    <t>капитан Шепард</t>
+  </si>
+  <si>
+    <t>СПЕКТР</t>
+  </si>
+  <si>
+    <t>Трисс Меригольд</t>
+  </si>
+  <si>
+    <t>жен</t>
+  </si>
+  <si>
+    <t>Геральт из Ривии</t>
+  </si>
+  <si>
+    <t>мужчина</t>
+  </si>
+  <si>
+    <t>исполнения всех желаний</t>
   </si>
 </sst>
 </file>
@@ -459,16 +483,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -519,8 +543,41 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -528,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E8FAB2-6777-4297-A3DB-429CB167C58E}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +605,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -562,7 +619,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -598,22 +655,22 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -634,18 +691,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add reading preferences from data file
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CongratulationsGenerator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7033F89-5222-4E2C-AC00-493AB12317B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B96C2A-D6F4-41C1-944D-C8FA905CEE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipients" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Коротков Иван</t>
   </si>
@@ -119,18 +119,9 @@
     <t>продвижения по карьерной лестнице</t>
   </si>
   <si>
-    <t>font</t>
-  </si>
-  <si>
-    <t>template</t>
-  </si>
-  <si>
     <t>Consolas</t>
   </si>
   <si>
-    <t>Congratulations letter template.dotx</t>
-  </si>
-  <si>
     <t>Оптимус Прайм</t>
   </si>
   <si>
@@ -156,6 +147,39 @@
   </si>
   <si>
     <t>исполнения всех желаний</t>
+  </si>
+  <si>
+    <t>Template.dotx</t>
+  </si>
+  <si>
+    <t>Font</t>
+  </si>
+  <si>
+    <t>Output path</t>
+  </si>
+  <si>
+    <t>Resources path</t>
+  </si>
+  <si>
+    <t>Default file name</t>
+  </si>
+  <si>
+    <t>Celebration name</t>
+  </si>
+  <si>
+    <t>C:\Projects\CongratulationsGenerator\Resources</t>
+  </si>
+  <si>
+    <t>C:\Projects\CongratulationsGenerator\Output</t>
+  </si>
+  <si>
+    <t>Letters</t>
+  </si>
+  <si>
+    <t>началом триместра</t>
+  </si>
+  <si>
+    <t>Template file</t>
   </si>
 </sst>
 </file>
@@ -545,34 +569,34 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E8FAB2-6777-4297-A3DB-429CB167C58E}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -655,7 +679,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -681,28 +705,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBA24F2-5634-40F0-B3CB-5E5C0BF1A3A9}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="60.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TODO note about auto saving and auto closing
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CongratulationsGenerator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B96C2A-D6F4-41C1-944D-C8FA905CEE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A697DD7-2422-4947-BE58-7B7B449DDAA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Коротков Иван</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Template file</t>
+  </si>
+  <si>
+    <t>Autoclose</t>
+  </si>
+  <si>
+    <t>Autosave</t>
   </si>
 </sst>
 </file>
@@ -705,10 +711,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBA24F2-5634-40F0-B3CB-5E5C0BF1A3A9}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,6 +770,22 @@
         <v>49</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add properties to configuration so they can be used instead of direct access to dictionary
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CongratulationsGenerator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A697DD7-2422-4947-BE58-7B7B449DDAA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ABDE86-AC3B-41BD-9485-6A946D0ACD51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipients" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Коротков Иван</t>
   </si>
@@ -180,12 +180,6 @@
   </si>
   <si>
     <t>Template file</t>
-  </si>
-  <si>
-    <t>Autoclose</t>
-  </si>
-  <si>
-    <t>Autosave</t>
   </si>
 </sst>
 </file>
@@ -711,10 +705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBA24F2-5634-40F0-B3CB-5E5C0BF1A3A9}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,22 +764,6 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>